<commit_message>
Módulo 10 - Gráficos dinanmicos
</commit_message>
<xml_diff>
--- a/módulo 10/aula-tabela-dinamica.xlsx
+++ b/módulo 10/aula-tabela-dinamica.xlsx
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId3"/>
+    <pivotCache cacheId="2" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8436" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8424" uniqueCount="28">
   <si>
     <t>DATA</t>
   </si>
@@ -120,28 +120,16 @@
     <t>Rótulos de Coluna</t>
   </si>
   <si>
-    <t>Soma de VALOR</t>
-  </si>
-  <si>
-    <t>Atualizar tabela dinamica: clica na tabela dinâmica/aba analisar/atualizar/atualizar</t>
-  </si>
-  <si>
     <t>Relatório de vendas por loja, gênero e categoria</t>
   </si>
   <si>
-    <t xml:space="preserve">Inserir segmentação: clica na tb dinâmica/analisar/inserir </t>
+    <t>Vendas (R$)</t>
   </si>
   <si>
-    <t>segmentação/seleciona os dados que deseja filtrar</t>
+    <t>Vendas (unidades)</t>
   </si>
   <si>
-    <t>Alinhar os objetos: Clica em uma segmentação/aperta ctrl e seleciona as outras</t>
-  </si>
-  <si>
-    <t>/aba opções/simbolode alinhar objetos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bloquear os blocos de segmentação:clica em qq lugar na tabela dinamica /analisar/tabela dinâmica/opções/desmarca a opção: Ajustar automaticamente das colunas ao atualizar  </t>
+    <t>Preço médio</t>
   </si>
 </sst>
 </file>
@@ -151,7 +139,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,6 +156,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -193,7 +189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -208,74 +204,27 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -447,6 +396,52 @@
       </fill>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -475,8 +470,8 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>1009650</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="2" name="LOJA"/>
@@ -493,7 +488,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -542,13 +537,13 @@
       <xdr:rowOff>95251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>847725</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="GÊNERO"/>
@@ -565,7 +560,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -619,8 +614,8 @@
       <xdr:row>1</xdr:row>
       <xdr:rowOff>1238251</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="4" name="CATEGORIA"/>
@@ -637,7 +632,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -687,12 +682,12 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>663575</xdr:colOff>
+      <xdr:colOff>396875</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>1066800</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="5" name="FORMA DE PAGAMENTO"/>
@@ -709,7 +704,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -758,7 +753,7 @@
   <cacheSource type="worksheet">
     <worksheetSource name="tbVendas"/>
   </cacheSource>
-  <cacheFields count="7">
+  <cacheFields count="8">
     <cacheField name="DATA" numFmtId="14">
       <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2016-12-31T00:00:00" maxDate="2018-10-31T00:00:00"/>
     </cacheField>
@@ -797,6 +792,7 @@
         <s v="Dinheiro"/>
       </sharedItems>
     </cacheField>
+    <cacheField name="Média" numFmtId="0" formula="VALOR /VOLUME" databaseField="0"/>
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
@@ -19712,9 +19708,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica2" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:F17" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabela dinâmica2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" colGrandTotals="0" itemPrintTitles="1" createdVersion="5" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:G10" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="8">
     <pivotField numFmtId="14" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="5">
@@ -19725,82 +19721,39 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisCol" showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="5">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="3"/>
-        <item x="2"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField axis="axisCol" showAll="0">
       <items count="3">
         <item x="0"/>
         <item x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
     <pivotField dataField="1" numFmtId="164" showAll="0"/>
     <pivotField multipleItemSelectionAllowed="1" showAll="0">
       <items count="4">
         <item x="2"/>
-        <item h="1" x="1"/>
-        <item h="1" x="0"/>
+        <item x="1"/>
+        <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
+    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
   <rowFields count="2">
+    <field x="2"/>
     <field x="1"/>
-    <field x="3"/>
   </rowFields>
-  <rowItems count="13">
-    <i>
-      <x/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="2"/>
-  </colFields>
-  <colItems count="5">
+  <rowItems count="5">
     <i>
       <x/>
     </i>
@@ -19816,11 +19769,39 @@
     <i t="grand">
       <x/>
     </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="3"/>
+    <field x="-2"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1" i="2">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1" i="1">
+      <x v="1"/>
+    </i>
+    <i r="1" i="2">
+      <x v="2"/>
+    </i>
   </colItems>
-  <dataFields count="1">
-    <dataField name="Soma de VALOR" fld="5" baseField="1" baseItem="1"/>
+  <dataFields count="3">
+    <dataField name="Vendas (R$)" fld="5" baseField="2" baseItem="0"/>
+    <dataField name="Vendas (unidades)" fld="4" baseField="2" baseItem="0"/>
+    <dataField name="Preço médio" fld="7" baseField="2" baseItem="0" numFmtId="2"/>
   </dataFields>
-  <pivotTableStyleInfo name="PivotStyleMedium14" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
@@ -19890,8 +19871,8 @@
     <tabular pivotCacheId="1">
       <items count="3">
         <i x="2" s="1"/>
-        <i x="1"/>
-        <i x="0"/>
+        <i x="1" s="1"/>
+        <i x="0" s="1"/>
       </items>
     </tabular>
   </data>
@@ -19902,22 +19883,22 @@
 <slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
   <slicer name="LOJA" cache="SegmentaçãodeDados_LOJA" caption="LOJA" columnCount="2" rowHeight="241300"/>
   <slicer name="GÊNERO" cache="SegmentaçãodeDados_GÊNERO" caption="GÊNERO" columnCount="2" rowHeight="241300"/>
-  <slicer name="CATEGORIA" cache="SegmentaçãodeDados_CATEGORIA" caption="CATEGORIA" columnCount="2" rowHeight="241300"/>
+  <slicer name="CATEGORIA" cache="SegmentaçãodeDados_CATEGORIA" caption="CATEGORIA" columnCount="2" style="SlicerStyleLight6" rowHeight="241300"/>
   <slicer name="FORMA DE PAGAMENTO" cache="SegmentaçãodeDados_FORMA_DE_PAGAMENTO" caption="FORMA DE PAGAMENTO" columnCount="2" rowHeight="241300"/>
 </slicers>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tbVendas" displayName="tbVendas" ref="A1:G2101" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="tbVendas" displayName="tbVendas" ref="A1:G2101" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G2101"/>
   <tableColumns count="7">
-    <tableColumn id="1" name="DATA" dataDxfId="8"/>
-    <tableColumn id="2" name="LOJA" dataDxfId="7"/>
-    <tableColumn id="3" name="CATEGORIA" dataDxfId="6"/>
-    <tableColumn id="4" name="GÊNERO" dataDxfId="5"/>
-    <tableColumn id="5" name="VOLUME" dataDxfId="4"/>
-    <tableColumn id="6" name="VALOR" dataDxfId="3"/>
-    <tableColumn id="7" name="FORMA DE PAGAMENTO" dataDxfId="2"/>
+    <tableColumn id="1" name="DATA" dataDxfId="6"/>
+    <tableColumn id="2" name="LOJA" dataDxfId="5"/>
+    <tableColumn id="3" name="CATEGORIA" dataDxfId="4"/>
+    <tableColumn id="4" name="GÊNERO" dataDxfId="3"/>
+    <tableColumn id="5" name="VOLUME" dataDxfId="2"/>
+    <tableColumn id="6" name="VALOR" dataDxfId="1"/>
+    <tableColumn id="7" name="FORMA DE PAGAMENTO" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -20220,263 +20201,278 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" style="11" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.5703125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.7109375" style="11" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="11" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="108" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="A1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:15" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13"/>
+      <c r="B2" s="13"/>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+    </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>24</v>
-      </c>
+      <c r="A3"/>
       <c r="B3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3" s="13"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4"/>
+      <c r="B4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+    </row>
+    <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="10">
-        <v>5308</v>
-      </c>
-      <c r="C5" s="10">
-        <v>7936</v>
-      </c>
-      <c r="D5" s="10">
-        <v>5278</v>
-      </c>
-      <c r="E5" s="10">
-        <v>9963</v>
-      </c>
-      <c r="F5" s="10">
-        <v>28485</v>
-      </c>
-      <c r="H5" s="13" t="s">
+      <c r="C5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="13"/>
-      <c r="K5" s="13"/>
-      <c r="L5" s="13"/>
-      <c r="M5" s="13"/>
-      <c r="N5" s="13"/>
-      <c r="O5" s="13"/>
+      <c r="E5" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5" s="10"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="10">
-        <v>3678</v>
-      </c>
-      <c r="C6" s="10">
-        <v>4017</v>
-      </c>
-      <c r="D6" s="10">
-        <v>3682</v>
-      </c>
-      <c r="E6" s="10">
-        <v>4784</v>
-      </c>
-      <c r="F6" s="10">
-        <v>16161</v>
-      </c>
-      <c r="H6" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
+        <v>8</v>
+      </c>
+      <c r="B6" s="8">
+        <v>44265</v>
+      </c>
+      <c r="C6" s="8">
+        <v>4218</v>
+      </c>
+      <c r="D6" s="15">
+        <v>10.494310099573257</v>
+      </c>
+      <c r="E6" s="8">
+        <v>35873</v>
+      </c>
+      <c r="F6" s="8">
+        <v>3481</v>
+      </c>
+      <c r="G6" s="15">
+        <v>10.305372019534616</v>
+      </c>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6" s="13"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="10">
-        <v>1630</v>
-      </c>
-      <c r="C7" s="10">
-        <v>3919</v>
-      </c>
-      <c r="D7" s="10">
-        <v>1596</v>
-      </c>
-      <c r="E7" s="10">
-        <v>5179</v>
-      </c>
-      <c r="F7" s="10">
-        <v>12324</v>
-      </c>
-      <c r="H7" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
+        <v>13</v>
+      </c>
+      <c r="B7" s="8">
+        <v>37763</v>
+      </c>
+      <c r="C7" s="8">
+        <v>3874</v>
+      </c>
+      <c r="D7" s="15">
+        <v>9.7478058853897789</v>
+      </c>
+      <c r="E7" s="8">
+        <v>50317</v>
+      </c>
+      <c r="F7" s="8">
+        <v>4808</v>
+      </c>
+      <c r="G7" s="15">
+        <v>10.465266222961731</v>
+      </c>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7" s="13"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="10">
-        <v>7208</v>
-      </c>
-      <c r="C8" s="10">
-        <v>8118</v>
-      </c>
-      <c r="D8" s="10">
-        <v>6733</v>
-      </c>
-      <c r="E8" s="10">
-        <v>8271</v>
-      </c>
-      <c r="F8" s="10">
-        <v>30330</v>
-      </c>
-      <c r="H8" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="8">
+        <v>39372</v>
+      </c>
+      <c r="C8" s="8">
+        <v>4005</v>
+      </c>
+      <c r="D8" s="15">
+        <v>9.8307116104868921</v>
+      </c>
+      <c r="E8" s="8">
+        <v>42080</v>
+      </c>
+      <c r="F8" s="8">
+        <v>3974</v>
+      </c>
+      <c r="G8" s="15">
+        <v>10.588827377956719</v>
+      </c>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8" s="13"/>
+    </row>
+    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="10">
-        <v>4071</v>
-      </c>
-      <c r="C9" s="10">
-        <v>3832</v>
-      </c>
-      <c r="D9" s="10">
-        <v>3716</v>
-      </c>
-      <c r="E9" s="10">
-        <v>2578</v>
-      </c>
-      <c r="F9" s="10">
-        <v>14197</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
+        <v>15</v>
+      </c>
+      <c r="B9" s="8">
+        <v>47813</v>
+      </c>
+      <c r="C9" s="8">
+        <v>4680</v>
+      </c>
+      <c r="D9" s="15">
+        <v>10.216452991452991</v>
+      </c>
+      <c r="E9" s="8">
+        <v>47319</v>
+      </c>
+      <c r="F9" s="8">
+        <v>4340</v>
+      </c>
+      <c r="G9" s="15">
+        <v>10.902995391705069</v>
+      </c>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
       <c r="O9" s="14"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="10">
-        <v>3137</v>
-      </c>
-      <c r="C10" s="10">
-        <v>4286</v>
-      </c>
-      <c r="D10" s="10">
-        <v>3017</v>
-      </c>
-      <c r="E10" s="10">
-        <v>5693</v>
-      </c>
-      <c r="F10" s="10">
-        <v>16133</v>
-      </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
-      <c r="L10" s="14"/>
-      <c r="M10" s="14"/>
-      <c r="N10" s="14"/>
+        <v>22</v>
+      </c>
+      <c r="B10" s="8">
+        <v>169213</v>
+      </c>
+      <c r="C10" s="8">
+        <v>16777</v>
+      </c>
+      <c r="D10" s="15">
+        <v>10.086010609763367</v>
+      </c>
+      <c r="E10" s="8">
+        <v>175589</v>
+      </c>
+      <c r="F10" s="8">
+        <v>16603</v>
+      </c>
+      <c r="G10" s="15">
+        <v>10.575739324218516</v>
+      </c>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
       <c r="O10" s="14"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="10">
-        <v>7192</v>
-      </c>
-      <c r="C11" s="10">
-        <v>5837</v>
-      </c>
-      <c r="D11" s="10">
-        <v>7063</v>
-      </c>
-      <c r="E11" s="10">
-        <v>6721</v>
-      </c>
-      <c r="F11" s="10">
-        <v>26813</v>
-      </c>
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="14"/>
@@ -20487,140 +20483,148 @@
       <c r="O11" s="14"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="10">
-        <v>3495</v>
-      </c>
-      <c r="C12" s="10">
-        <v>2886</v>
-      </c>
-      <c r="D12" s="10">
-        <v>3936</v>
-      </c>
-      <c r="E12" s="10">
-        <v>3353</v>
-      </c>
-      <c r="F12" s="10">
-        <v>13670</v>
-      </c>
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="10">
-        <v>3697</v>
-      </c>
-      <c r="C13" s="10">
-        <v>2951</v>
-      </c>
-      <c r="D13" s="10">
-        <v>3127</v>
-      </c>
-      <c r="E13" s="10">
-        <v>3368</v>
-      </c>
-      <c r="F13" s="10">
-        <v>13143</v>
-      </c>
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="10">
-        <v>6326</v>
-      </c>
-      <c r="C14" s="10">
-        <v>5149</v>
-      </c>
-      <c r="D14" s="10">
-        <v>8064</v>
-      </c>
-      <c r="E14" s="10">
-        <v>6195</v>
-      </c>
-      <c r="F14" s="10">
-        <v>25734</v>
-      </c>
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" s="10">
-        <v>4711</v>
-      </c>
-      <c r="C15" s="10">
-        <v>1354</v>
-      </c>
-      <c r="D15" s="10">
-        <v>3263</v>
-      </c>
-      <c r="E15" s="10">
-        <v>3700</v>
-      </c>
-      <c r="F15" s="10">
-        <v>13028</v>
-      </c>
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="10">
-        <v>1615</v>
-      </c>
-      <c r="C16" s="10">
-        <v>3795</v>
-      </c>
-      <c r="D16" s="10">
-        <v>4801</v>
-      </c>
-      <c r="E16" s="10">
-        <v>2495</v>
-      </c>
-      <c r="F16" s="10">
-        <v>12706</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="10">
-        <v>26034</v>
-      </c>
-      <c r="C17" s="10">
-        <v>27040</v>
-      </c>
-      <c r="D17" s="10">
-        <v>27138</v>
-      </c>
-      <c r="E17" s="10">
-        <v>31150</v>
-      </c>
-      <c r="F17" s="10">
-        <v>111362</v>
-      </c>
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="H3:O3"/>
-    <mergeCell ref="H5:O5"/>
-    <mergeCell ref="H6:O6"/>
-    <mergeCell ref="H7:O7"/>
-    <mergeCell ref="H8:O8"/>
-    <mergeCell ref="H9:O11"/>
-  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
       <x14:slicerList>
-        <x14:slicer r:id="rId3"/>
+        <x14:slicer r:id="rId4"/>
       </x14:slicerList>
     </ext>
   </extLst>
@@ -20632,7 +20636,7 @@
   <dimension ref="A1:J2101"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>